<commit_message>
mise à jour du repo avec l'ajout de 3 projets en lien avec les frameworks CSS
</commit_message>
<xml_diff>
--- a/Challenges of the week.xlsx
+++ b/Challenges of the week.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loic8\Bureau\Formations\BeCode\challenges-of-the-week\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB52521E-6F36-4753-BC3D-94FBF36F6C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4E971C-5281-452C-88DA-A96E4BCDF7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{3F5598A8-3A1E-4FFD-8CE0-C347D8B5DC8D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Mes challenges of the week </t>
   </si>
@@ -48,10 +48,19 @@
     <t xml:space="preserve">Revoir git sur https://www.w3schools.com/git/default.asp?remote=github </t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Faire un site respectant ARIA et accessibilité</t>
+  </si>
+  <si>
+    <t>Faire un site en utilisant SASS (projet 1)</t>
+  </si>
+  <si>
+    <t>Faire un site en utilisant SASS + responsive (projet 1)</t>
+  </si>
+  <si>
+    <t>Utiliser des framework pour réaliser une landing page (Projet 2), un site e-commerce (Projet 3) et une boite mail (Projet 4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faire un projet pro pour un cv déployable sur LinkedIn </t>
   </si>
 </sst>
 </file>
@@ -460,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58078BB7-7C6D-4497-A1F0-166F5D1D4A33}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -503,7 +512,7 @@
         <v>44606</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -511,12 +520,31 @@
         <v>44613</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>44620</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>44626</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>44626</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajout du challenge de la semaine
</commit_message>
<xml_diff>
--- a/Challenges of the week.xlsx
+++ b/Challenges of the week.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loic8\Bureau\Formations\BeCode\challenges-of-the-week\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4E971C-5281-452C-88DA-A96E4BCDF7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512CB66F-5FBD-47B1-91B0-3246B1591ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{3F5598A8-3A1E-4FFD-8CE0-C347D8B5DC8D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t xml:space="preserve">Mes challenges of the week </t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t xml:space="preserve">Faire un projet pro pour un cv déployable sur LinkedIn </t>
+  </si>
+  <si>
+    <t>Ecriture aide-mémoire Javascript</t>
   </si>
 </sst>
 </file>
@@ -469,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58078BB7-7C6D-4497-A1F0-166F5D1D4A33}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="B10" sqref="B10:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -533,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>44626</v>
+        <v>44627</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
@@ -541,10 +544,26 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>44626</v>
+        <v>44627</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>44634</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>44641</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>